<commit_message>
feat: added rating flag
</commit_message>
<xml_diff>
--- a/test_data_file.xlsx
+++ b/test_data_file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>Player</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Alan</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>Aaron</t>
   </si>
   <si>
@@ -83,9 +86,6 @@
   </si>
   <si>
     <t>Abdullah</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Anton</t>
@@ -118,7 +118,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -164,10 +164,10 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -524,13 +524,13 @@
       <c r="B3" s="3">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>4</v>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3">
         <v>8</v>
@@ -541,18 +541,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>4</v>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -563,7 +563,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -574,18 +574,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>4</v>
+      <c r="C8" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3">
         <v>2</v>
@@ -596,7 +596,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3">
         <v>3</v>
@@ -607,18 +607,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3">
         <v>4</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3">
         <v>5</v>
@@ -629,18 +629,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3">
         <v>6</v>
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="5">
+        <v>17</v>
+      </c>
+      <c r="B14" s="6">
         <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -649,7 +649,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" s="3">
         <v>8</v>
@@ -660,16 +660,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -680,7 +682,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3">
         <v>4</v>
@@ -691,7 +693,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19" s="3">
         <v>8</v>
@@ -702,13 +704,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" s="3">
         <v>9</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>23</v>
+      <c r="C20" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
@@ -729,8 +731,8 @@
       <c r="B22" s="7">
         <v>3.4</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>4</v>
+      <c r="C22" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">

</xml_diff>